<commit_message>
blog dan comment belom!!
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\fano2.11_CI_KOYOS\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26831C1F-F8EE-41DA-831A-CCFA50498B0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD43753-ED94-4627-AC5A-09B211F25685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="32">
   <si>
     <t>foto</t>
   </si>
@@ -106,19 +106,16 @@
     <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry.</t>
   </si>
   <si>
-    <t>Nyoba aja</t>
+    <t>http://localhost/fano2.11_CI_KOYOS/inti/images/photo.png</t>
   </si>
   <si>
-    <t>Nyoba doang</t>
+    <t>nyoba_aja</t>
   </si>
   <si>
-    <t>Nyoba atuh</t>
+    <t>nyoba_doang</t>
   </si>
   <si>
-    <t>Nyoba yaaa</t>
-  </si>
-  <si>
-    <t>http://localhost/fano2.11_CI_KOYOS/inti/images/photo.png</t>
+    <t>nyoba_1</t>
   </si>
 </sst>
 </file>
@@ -559,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D49"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,22 +679,22 @@
         <v>27</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -741,22 +738,22 @@
         <v>28</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -800,22 +797,22 @@
         <v>29</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -859,22 +856,22 @@
         <v>30</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -918,22 +915,22 @@
         <v>31</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -977,22 +974,22 @@
         <v>32</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1036,22 +1033,22 @@
         <v>33</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1095,22 +1092,22 @@
         <v>34</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1157,19 +1154,19 @@
         <v>29</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1216,19 +1213,19 @@
         <v>29</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1275,19 +1272,19 @@
         <v>29</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1334,19 +1331,19 @@
         <v>29</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1393,19 +1390,19 @@
         <v>29</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1452,19 +1449,19 @@
         <v>29</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1511,19 +1508,19 @@
         <v>29</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1570,19 +1567,19 @@
         <v>29</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1629,19 +1626,19 @@
         <v>29</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S18" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1688,19 +1685,19 @@
         <v>29</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1744,22 +1741,22 @@
         <v>45</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1803,22 +1800,22 @@
         <v>46</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S21" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1862,22 +1859,22 @@
         <v>47</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1921,22 +1918,22 @@
         <v>48</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1980,22 +1977,22 @@
         <v>49</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2039,22 +2036,22 @@
         <v>50</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S25" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2101,19 +2098,19 @@
         <v>30</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P26" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R26" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S26" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2160,19 +2157,19 @@
         <v>30</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S27" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2219,19 +2216,19 @@
         <v>30</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2278,19 +2275,19 @@
         <v>30</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P29" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S29" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2337,19 +2334,19 @@
         <v>30</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P30" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q30" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S30" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2396,19 +2393,19 @@
         <v>30</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P31" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q31" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R31" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S31" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2455,19 +2452,19 @@
         <v>30</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P32" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S32" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2514,19 +2511,19 @@
         <v>30</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q33" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R33" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S33" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2573,19 +2570,19 @@
         <v>30</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P34" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q34" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R34" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S34" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2632,19 +2629,19 @@
         <v>30</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q35" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R35" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S35" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2691,19 +2688,19 @@
         <v>30</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q36" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R36" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S36" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2750,19 +2747,19 @@
         <v>30</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q37" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R37" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S37" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2809,19 +2806,19 @@
         <v>30</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q38" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R38" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S38" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2868,19 +2865,19 @@
         <v>30</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q39" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R39" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S39" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2927,19 +2924,19 @@
         <v>30</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P40" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q40" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R40" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S40" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -2986,19 +2983,19 @@
         <v>30</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P41" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R41" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S41" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -3045,19 +3042,19 @@
         <v>30</v>
       </c>
       <c r="O42" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P42" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R42" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S42" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -3104,19 +3101,19 @@
         <v>30</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P43" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q43" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S43" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -3163,19 +3160,19 @@
         <v>30</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q44" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R44" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S44" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -3222,19 +3219,19 @@
         <v>30</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P45" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q45" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R45" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S45" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -3281,19 +3278,19 @@
         <v>30</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P46" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q46" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R46" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S46" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -3337,22 +3334,22 @@
         <v>72</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P47" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q47" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S47" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -3396,22 +3393,22 @@
         <v>73</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P48" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q48" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S48" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="225" x14ac:dyDescent="0.25">
@@ -3458,19 +3455,19 @@
         <v>31</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P49" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q49" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R49" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S49" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>